<commit_message>
Risk 13.0.1 Installment Payments
</commit_message>
<xml_diff>
--- a/Risk.xlsx
+++ b/Risk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\AI\Risk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EC040D-4141-47C6-A5FE-EF1BA28F977A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4A43D5-BAD2-4A8F-8EDA-DD8E80E15818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="380" windowWidth="19200" windowHeight="10200" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ideas" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Risk 5.0 Engineering" sheetId="16" r:id="rId7"/>
     <sheet name="Risk 6.0 Preparation" sheetId="17" r:id="rId8"/>
     <sheet name="Risk 7.0 LightGBM" sheetId="18" r:id="rId9"/>
-    <sheet name="Risk 8.0 Reduction" sheetId="23" r:id="rId10"/>
+    <sheet name="Risk 8.0 Elimination" sheetId="23" r:id="rId10"/>
     <sheet name="Risk 10.0 EDA" sheetId="14" r:id="rId11"/>
     <sheet name="Risk 11.0 Bureau" sheetId="19" r:id="rId12"/>
     <sheet name="Risk 12.0 Applications" sheetId="20" r:id="rId13"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="136">
   <si>
     <t>Version</t>
   </si>
@@ -299,9 +299,6 @@
     <t>WoE Encoder-- Feature Engine Library</t>
   </si>
   <si>
-    <t>Ater Random Sample Imputer, correlation of Ext_Source_1 and Target went down significantly.</t>
-  </si>
-  <si>
     <t>Risk 2.0.2</t>
   </si>
   <si>
@@ -360,9 +357,6 @@
   </si>
   <si>
     <t>Risk 6.0.0</t>
-  </si>
-  <si>
-    <t>10.1.1</t>
   </si>
   <si>
     <t>LightGBM</t>
@@ -444,6 +438,33 @@
   </si>
   <si>
     <t>Applications</t>
+  </si>
+  <si>
+    <t>After Random Sample Imputer, correlation of Ext_Source_1 and Target went down significantly.</t>
+  </si>
+  <si>
+    <t>Risk 10.1.1</t>
+  </si>
+  <si>
+    <t>Risk 13.0.0</t>
+  </si>
+  <si>
+    <t>2024 10 03</t>
+  </si>
+  <si>
+    <t>Installment Began from 12.5.1</t>
+  </si>
+  <si>
+    <t>Risk 4.0.0</t>
+  </si>
+  <si>
+    <t>Went from 122 features to 83 features.</t>
+  </si>
+  <si>
+    <t>Impute by a specific number using Feature Engine Library</t>
+  </si>
+  <si>
+    <t>Drop Constant Features on app_train using Feature Engine Library</t>
   </si>
 </sst>
 </file>
@@ -1473,10 +1494,10 @@
     </row>
     <row r="47" spans="1:11">
       <c r="B47" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -4331,7 +4352,7 @@
   <dimension ref="A1:L986"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4361,16 +4382,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -4379,7 +4400,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -4393,10 +4414,6 @@
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:9">
@@ -7468,7 +7485,7 @@
   <dimension ref="A1:L986"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7520,16 +7537,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -7540,7 +7557,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -7549,7 +7566,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -7562,13 +7579,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -13747,7 +13764,7 @@
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:L987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -13778,16 +13795,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -13800,16 +13817,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -13820,7 +13837,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -13829,7 +13846,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -13842,16 +13859,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -13860,7 +13877,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -16912,7 +16929,7 @@
   <dimension ref="A1:L986"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16941,10 +16958,18 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:9">
@@ -22624,7 +22649,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="30"/>
       <c r="D6" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -22696,7 +22721,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -25880,16 +25905,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -28971,7 +28996,7 @@
   <dimension ref="A1:L986"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -29052,7 +29077,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -29065,7 +29090,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>77</v>
@@ -29074,7 +29099,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -29087,16 +29112,16 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="5"/>
     </row>
@@ -29109,16 +29134,16 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="5"/>
     </row>
@@ -29126,7 +29151,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
       <c r="D13" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G13" s="5"/>
     </row>
@@ -29138,16 +29163,16 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -32188,7 +32213,7 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -35283,8 +35308,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:L986"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -35313,17 +35338,27 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:9">
@@ -35339,7 +35374,9 @@
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:9">
@@ -38441,13 +38478,13 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
       <c r="A2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3"/>
       <c r="G2" s="5"/>
@@ -41574,13 +41611,13 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3"/>
       <c r="G2" s="5"/>
@@ -44707,16 +44744,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
       <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -44729,16 +44766,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3"/>
@@ -44749,7 +44786,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -44758,7 +44795,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G6" s="5"/>
     </row>

</xml_diff>